<commit_message>
added new data, create a test for tkinter
</commit_message>
<xml_diff>
--- a/Perry Tables.xlsx
+++ b/Perry Tables.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aipry\PycharmProjects\perrigrin\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aipry\PycharmProjects\pythochem\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{A381F3F0-52C8-454D-B44F-1C9B0BED4CC1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14701C5F-1DDE-4305-9E78-D6C320FC76D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{772E457C-031C-44CE-B0C6-9E682C413415}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="273" uniqueCount="108">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="644" uniqueCount="287">
   <si>
     <t>Length</t>
   </si>
@@ -360,6 +360,543 @@
   </si>
   <si>
     <t>Volume/length (linear displacement)</t>
+  </si>
+  <si>
+    <t>Amount of substance</t>
+  </si>
+  <si>
+    <t>lbm-mol</t>
+  </si>
+  <si>
+    <t>kmol</t>
+  </si>
+  <si>
+    <t>std m3(0°C, 1 atm)</t>
+  </si>
+  <si>
+    <t>std fi3 (60°F, 1 atm)</t>
+  </si>
+  <si>
+    <t>Btu/lbm</t>
+  </si>
+  <si>
+    <t>MJ/kg</t>
+  </si>
+  <si>
+    <t>kJ/kg</t>
+  </si>
+  <si>
+    <t>J/g</t>
+  </si>
+  <si>
+    <t>kWh/kg</t>
+  </si>
+  <si>
+    <t>cal/g</t>
+  </si>
+  <si>
+    <t>cal/lbm</t>
+  </si>
+  <si>
+    <t>J/kg</t>
+  </si>
+  <si>
+    <t>kcal/(g.mol)</t>
+  </si>
+  <si>
+    <t>kJ/kmol</t>
+  </si>
+  <si>
+    <t>Btu/(lb-mol)</t>
+  </si>
+  <si>
+    <t>Btu/U.S. gal</t>
+  </si>
+  <si>
+    <t>MJ/m³</t>
+  </si>
+  <si>
+    <t>kJ/dm³</t>
+  </si>
+  <si>
+    <t>kJ/m³</t>
+  </si>
+  <si>
+    <t>kWh/m³</t>
+  </si>
+  <si>
+    <t>Btu/U.K. gal</t>
+  </si>
+  <si>
+    <t>kJ/m3</t>
+  </si>
+  <si>
+    <t>Btu/ft3</t>
+  </si>
+  <si>
+    <t>kJ/dm3</t>
+  </si>
+  <si>
+    <t>kWh/m3</t>
+  </si>
+  <si>
+    <t>cal/mL</t>
+  </si>
+  <si>
+    <t>(ft.lbf)/U.S. gal</t>
+  </si>
+  <si>
+    <t>J/dm³</t>
+  </si>
+  <si>
+    <t>kcal/m3</t>
+  </si>
+  <si>
+    <t>Specific entropy</t>
+  </si>
+  <si>
+    <t>Btu/(lbm.°R)</t>
+  </si>
+  <si>
+    <t>kJ/(kg.K)</t>
+  </si>
+  <si>
+    <t>J/(g.K)</t>
+  </si>
+  <si>
+    <t>cal/(g.K)</t>
+  </si>
+  <si>
+    <t>kJ/(kg-K)</t>
+  </si>
+  <si>
+    <t>kcal/(kg.°C)</t>
+  </si>
+  <si>
+    <t>kWh/(kg.°C)</t>
+  </si>
+  <si>
+    <t>Btu/(lbm-°F)</t>
+  </si>
+  <si>
+    <t>J/(g-K)</t>
+  </si>
+  <si>
+    <t>Btu/(lb-mol.°F)</t>
+  </si>
+  <si>
+    <t>kJ/(kmol-K)</t>
+  </si>
+  <si>
+    <t>cal/(g.mol.°C)</t>
+  </si>
+  <si>
+    <t>Temperature, pressure, vacuum</t>
+  </si>
+  <si>
+    <t>Temperature (absolute)</t>
+  </si>
+  <si>
+    <t>°R</t>
+  </si>
+  <si>
+    <t>K</t>
+  </si>
+  <si>
+    <t>Temperature (traditional)</t>
+  </si>
+  <si>
+    <t>°F</t>
+  </si>
+  <si>
+    <t>°C</t>
+  </si>
+  <si>
+    <t>Temperature (difference)</t>
+  </si>
+  <si>
+    <t>K, °C</t>
+  </si>
+  <si>
+    <t>Pressure</t>
+  </si>
+  <si>
+    <t>atm (760 mmHg at 0°C or 14,696 psi)</t>
+  </si>
+  <si>
+    <t>MPa</t>
+  </si>
+  <si>
+    <t>kPa</t>
+  </si>
+  <si>
+    <t>bar</t>
+  </si>
+  <si>
+    <t>mmHg (0°C) = torr</t>
+  </si>
+  <si>
+    <t>umHg (0°C)</t>
+  </si>
+  <si>
+    <t>ubar</t>
+  </si>
+  <si>
+    <t>mmHg = torr (0°C)</t>
+  </si>
+  <si>
+    <t>cmH2O (4°C)</t>
+  </si>
+  <si>
+    <t>lbf/ft2 (psf)</t>
+  </si>
+  <si>
+    <t>mHg (0°C)</t>
+  </si>
+  <si>
+    <t>Pa</t>
+  </si>
+  <si>
+    <t>dyn/cm2</t>
+  </si>
+  <si>
+    <t>Vacuum, draft</t>
+  </si>
+  <si>
+    <t>inHg (60°F)</t>
+  </si>
+  <si>
+    <t>inH2O (39.2°F)</t>
+  </si>
+  <si>
+    <t>inH2O (60°F)</t>
+  </si>
+  <si>
+    <t>Liquid head</t>
+  </si>
+  <si>
+    <t>Pressure drop/length</t>
+  </si>
+  <si>
+    <t>psi/ft</t>
+  </si>
+  <si>
+    <t>kPa/m</t>
+  </si>
+  <si>
+    <t>Calorific value, enthalpy (mass basis)</t>
+  </si>
+  <si>
+    <t>Caloric value, enthalpy (mole basis)</t>
+  </si>
+  <si>
+    <t>Calorific value (volume basis-solids and liquids)</t>
+  </si>
+  <si>
+    <t>Calorific value (volume basis-gases)</t>
+  </si>
+  <si>
+    <t>Specific-heat capacity (mass basis)</t>
+  </si>
+  <si>
+    <t>Specific-heat capacity (mole basis)</t>
+  </si>
+  <si>
+    <t>Enthalpy, calorific value, heat, entropy, heat capacity</t>
+  </si>
+  <si>
+    <t>(°F − 32)*5/9</t>
+  </si>
+  <si>
+    <t>°F*5/9</t>
+  </si>
+  <si>
+    <t>°R*5/9</t>
+  </si>
+  <si>
+    <t>batch 2</t>
+  </si>
+  <si>
+    <t>Density</t>
+  </si>
+  <si>
+    <t>lbm/ft</t>
+  </si>
+  <si>
+    <t>kg/m³</t>
+  </si>
+  <si>
+    <t>g/m³</t>
+  </si>
+  <si>
+    <t>lbm/U.S. gal</t>
+  </si>
+  <si>
+    <t>g/cm³</t>
+  </si>
+  <si>
+    <t>lbm/U.K. gal</t>
+  </si>
+  <si>
+    <t>lbm/ft3</t>
+  </si>
+  <si>
+    <t>Specific volume</t>
+  </si>
+  <si>
+    <t>ft3/lbm</t>
+  </si>
+  <si>
+    <t>m3/kg</t>
+  </si>
+  <si>
+    <t>m3//g</t>
+  </si>
+  <si>
+    <t>dm3/kg</t>
+  </si>
+  <si>
+    <t>U.K. gal/lbm</t>
+  </si>
+  <si>
+    <t>cm3/g</t>
+  </si>
+  <si>
+    <t>U.S. gal/lbm</t>
+  </si>
+  <si>
+    <t>Specific volume (mole basis)</t>
+  </si>
+  <si>
+    <t>L/(g.mol)</t>
+  </si>
+  <si>
+    <t>m3/kmol</t>
+  </si>
+  <si>
+    <t>ft3/(lb-mol)</t>
+  </si>
+  <si>
+    <t>bbl/U.S. ton</t>
+  </si>
+  <si>
+    <t>m3/t</t>
+  </si>
+  <si>
+    <t>bbl/U.K. ton</t>
+  </si>
+  <si>
+    <t>Yield</t>
+  </si>
+  <si>
+    <t>dm3/t</t>
+  </si>
+  <si>
+    <t>L/t</t>
+  </si>
+  <si>
+    <t>U.S. gal/U.S. ton</t>
+  </si>
+  <si>
+    <t>dm 3//t</t>
+  </si>
+  <si>
+    <t>U.S. gal/U.K. ton</t>
+  </si>
+  <si>
+    <t>Concentration (mass/mass)</t>
+  </si>
+  <si>
+    <t>wt %</t>
+  </si>
+  <si>
+    <t>kg/kg</t>
+  </si>
+  <si>
+    <t>g/kg</t>
+  </si>
+  <si>
+    <t>wt ppm</t>
+  </si>
+  <si>
+    <t>mg/kg</t>
+  </si>
+  <si>
+    <t>Concentration (mass/volume)</t>
+  </si>
+  <si>
+    <t>lbm/bbl</t>
+  </si>
+  <si>
+    <t>g/dm³</t>
+  </si>
+  <si>
+    <t>g/U.S. gal</t>
+  </si>
+  <si>
+    <t>g/U.K. gal</t>
+  </si>
+  <si>
+    <t>g/L</t>
+  </si>
+  <si>
+    <t>lbm/1000 U.S. gal</t>
+  </si>
+  <si>
+    <t>g/m3</t>
+  </si>
+  <si>
+    <t>mg/dm³</t>
+  </si>
+  <si>
+    <t>lbm/1000 U.K. gal</t>
+  </si>
+  <si>
+    <t>gr/U.S. gal</t>
+  </si>
+  <si>
+    <t>gr/ft³</t>
+  </si>
+  <si>
+    <t>mg/m³</t>
+  </si>
+  <si>
+    <t>lbm/1000 bbl</t>
+  </si>
+  <si>
+    <t>mg/U.S. gal</t>
+  </si>
+  <si>
+    <t>gr/100 ft</t>
+  </si>
+  <si>
+    <t>Concentration (volume/volume)</t>
+  </si>
+  <si>
+    <t>ft3/ft3</t>
+  </si>
+  <si>
+    <t>m3//m³</t>
+  </si>
+  <si>
+    <t>bbl/(acre-ft)</t>
+  </si>
+  <si>
+    <t>m3//3³</t>
+  </si>
+  <si>
+    <t>vol%</t>
+  </si>
+  <si>
+    <t>U.K. gal/ft3</t>
+  </si>
+  <si>
+    <t>dm³/Superscript(3)</t>
+  </si>
+  <si>
+    <t>L/m³</t>
+  </si>
+  <si>
+    <t>U.S. gal/ft3</t>
+  </si>
+  <si>
+    <t>mL/U.S. gal</t>
+  </si>
+  <si>
+    <t>mL/U.K. gal</t>
+  </si>
+  <si>
+    <t>vol ppm</t>
+  </si>
+  <si>
+    <t>cm³/m</t>
+  </si>
+  <si>
+    <t>U.K. gal/1000 bbl</t>
+  </si>
+  <si>
+    <t>U.S. gal/1000 bbl</t>
+  </si>
+  <si>
+    <t>U.K. pt/1000 bbl</t>
+  </si>
+  <si>
+    <t>Concentration (mole/volume)</t>
+  </si>
+  <si>
+    <t>(lb-mol)/U.S. gal</t>
+  </si>
+  <si>
+    <t>kmol/m³</t>
+  </si>
+  <si>
+    <t>(lb-mol)/U.K. gal</t>
+  </si>
+  <si>
+    <t>(lb.mol)/ft3</t>
+  </si>
+  <si>
+    <t>std ft3 (60°F, 1 atm)/bbl</t>
+  </si>
+  <si>
+    <t>Concentration (volume/mole)</t>
+  </si>
+  <si>
+    <t>U.S. gal/1000 std ft3 (60°F/60°F)</t>
+  </si>
+  <si>
+    <t>dm3/kmol</t>
+  </si>
+  <si>
+    <t>L/kmol</t>
+  </si>
+  <si>
+    <t>bbl/million std ft3 (60°F/60°F)</t>
+  </si>
+  <si>
+    <t>Facility throughput, capacity</t>
+  </si>
+  <si>
+    <t>Throughput (mass basis)</t>
+  </si>
+  <si>
+    <t>U.K. ton/year</t>
+  </si>
+  <si>
+    <t>t/a</t>
+  </si>
+  <si>
+    <t>U.S. ton/year</t>
+  </si>
+  <si>
+    <t>U.K. ton/day</t>
+  </si>
+  <si>
+    <t>t/d</t>
+  </si>
+  <si>
+    <t>t/h</t>
+  </si>
+  <si>
+    <t>U.S. ton/day</t>
+  </si>
+  <si>
+    <t>U.K. ton/h</t>
+  </si>
+  <si>
+    <t>U.S. ton/h</t>
+  </si>
+  <si>
+    <t>lbm/h</t>
+  </si>
+  <si>
+    <t>kg/h</t>
+  </si>
+  <si>
+    <t>Density, specific volume, concentration, dosage</t>
+  </si>
+  <si>
+    <t>batch 3</t>
   </si>
 </sst>
 </file>
@@ -375,12 +912,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -395,8 +938,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -711,16 +1255,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D1F4B472-F098-4375-8DA3-8F6E097903F5}">
-  <dimension ref="A1:F68"/>
+  <dimension ref="A1:G192"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+    <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
+      <selection activeCell="B69" sqref="B69"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="23.5546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="18.77734375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.5546875" customWidth="1"/>
     <col min="6" max="6" width="20" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1848,7 +2393,7 @@
         <v>45.35924</v>
       </c>
     </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
         <v>91</v>
       </c>
@@ -1865,7 +2410,7 @@
         <v>0.453592</v>
       </c>
     </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
         <v>91</v>
       </c>
@@ -1882,7 +2427,7 @@
         <v>31.103480000000001</v>
       </c>
     </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
         <v>91</v>
       </c>
@@ -1899,7 +2444,7 @@
         <v>28.349499999999999</v>
       </c>
     </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
         <v>91</v>
       </c>
@@ -1914,6 +2459,2328 @@
       </c>
       <c r="F68">
         <v>64.798910000000006</v>
+      </c>
+    </row>
+    <row r="69" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A69" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="B69" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="C69" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="D69" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="E69" s="1"/>
+      <c r="F69" s="1">
+        <v>0.45359240000000001</v>
+      </c>
+      <c r="G69" s="1" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="70" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A70" t="s">
+        <v>91</v>
+      </c>
+      <c r="B70" t="s">
+        <v>108</v>
+      </c>
+      <c r="C70" t="s">
+        <v>111</v>
+      </c>
+      <c r="D70" t="s">
+        <v>110</v>
+      </c>
+      <c r="F70">
+        <v>4.4615799999999997E-2</v>
+      </c>
+    </row>
+    <row r="71" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A71" t="s">
+        <v>91</v>
+      </c>
+      <c r="B71" t="s">
+        <v>108</v>
+      </c>
+      <c r="C71" t="s">
+        <v>112</v>
+      </c>
+      <c r="D71" t="s">
+        <v>110</v>
+      </c>
+      <c r="F71">
+        <v>1.1953000000000001E-3</v>
+      </c>
+    </row>
+    <row r="72" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A72" t="s">
+        <v>188</v>
+      </c>
+      <c r="B72" t="s">
+        <v>182</v>
+      </c>
+      <c r="C72" t="s">
+        <v>113</v>
+      </c>
+      <c r="D72" t="s">
+        <v>114</v>
+      </c>
+      <c r="F72">
+        <v>2.3259999999999999E-3</v>
+      </c>
+    </row>
+    <row r="73" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A73" t="s">
+        <v>188</v>
+      </c>
+      <c r="B73" t="s">
+        <v>182</v>
+      </c>
+      <c r="D73" t="s">
+        <v>115</v>
+      </c>
+      <c r="E73" t="s">
+        <v>116</v>
+      </c>
+      <c r="F73">
+        <v>2.3260000000000001</v>
+      </c>
+    </row>
+    <row r="74" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A74" t="s">
+        <v>188</v>
+      </c>
+      <c r="B74" t="s">
+        <v>182</v>
+      </c>
+      <c r="D74" t="s">
+        <v>117</v>
+      </c>
+      <c r="F74">
+        <v>6.4611119999999995E-4</v>
+      </c>
+    </row>
+    <row r="75" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A75" t="s">
+        <v>188</v>
+      </c>
+      <c r="B75" t="s">
+        <v>182</v>
+      </c>
+      <c r="C75" t="s">
+        <v>118</v>
+      </c>
+      <c r="D75" t="s">
+        <v>115</v>
+      </c>
+      <c r="E75" t="s">
+        <v>116</v>
+      </c>
+      <c r="F75">
+        <v>4.1840000000000002</v>
+      </c>
+    </row>
+    <row r="76" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A76" t="s">
+        <v>188</v>
+      </c>
+      <c r="B76" t="s">
+        <v>182</v>
+      </c>
+      <c r="C76" t="s">
+        <v>119</v>
+      </c>
+      <c r="D76" t="s">
+        <v>120</v>
+      </c>
+      <c r="F76">
+        <v>9.2241409999999995</v>
+      </c>
+    </row>
+    <row r="77" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A77" t="s">
+        <v>188</v>
+      </c>
+      <c r="B77" t="s">
+        <v>183</v>
+      </c>
+      <c r="C77" t="s">
+        <v>121</v>
+      </c>
+      <c r="D77" t="s">
+        <v>122</v>
+      </c>
+      <c r="F77">
+        <v>4184</v>
+      </c>
+    </row>
+    <row r="78" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A78" t="s">
+        <v>188</v>
+      </c>
+      <c r="B78" t="s">
+        <v>183</v>
+      </c>
+      <c r="C78" t="s">
+        <v>123</v>
+      </c>
+      <c r="D78" t="s">
+        <v>122</v>
+      </c>
+      <c r="F78">
+        <v>2.3260000000000001</v>
+      </c>
+    </row>
+    <row r="79" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A79" t="s">
+        <v>188</v>
+      </c>
+      <c r="B79" t="s">
+        <v>184</v>
+      </c>
+      <c r="C79" t="s">
+        <v>124</v>
+      </c>
+      <c r="D79" t="s">
+        <v>125</v>
+      </c>
+      <c r="E79" t="s">
+        <v>126</v>
+      </c>
+      <c r="F79">
+        <v>0.27871629999999997</v>
+      </c>
+    </row>
+    <row r="80" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A80" t="s">
+        <v>188</v>
+      </c>
+      <c r="B80" t="s">
+        <v>184</v>
+      </c>
+      <c r="D80" t="s">
+        <v>127</v>
+      </c>
+      <c r="F80">
+        <v>278.71629999999999</v>
+      </c>
+    </row>
+    <row r="81" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A81" t="s">
+        <v>188</v>
+      </c>
+      <c r="B81" t="s">
+        <v>184</v>
+      </c>
+      <c r="D81" t="s">
+        <v>128</v>
+      </c>
+      <c r="F81">
+        <v>7.7421100000000007E-2</v>
+      </c>
+    </row>
+    <row r="82" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A82" t="s">
+        <v>188</v>
+      </c>
+      <c r="B82" t="s">
+        <v>184</v>
+      </c>
+      <c r="C82" t="s">
+        <v>129</v>
+      </c>
+      <c r="D82" t="s">
+        <v>125</v>
+      </c>
+      <c r="E82" t="s">
+        <v>126</v>
+      </c>
+      <c r="F82">
+        <v>0.23208000000000001</v>
+      </c>
+    </row>
+    <row r="83" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A83" t="s">
+        <v>188</v>
+      </c>
+      <c r="B83" t="s">
+        <v>184</v>
+      </c>
+      <c r="D83" t="s">
+        <v>130</v>
+      </c>
+      <c r="F83">
+        <v>232.08</v>
+      </c>
+    </row>
+    <row r="84" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A84" t="s">
+        <v>188</v>
+      </c>
+      <c r="B84" t="s">
+        <v>184</v>
+      </c>
+      <c r="C84" t="s">
+        <v>131</v>
+      </c>
+      <c r="D84" t="s">
+        <v>128</v>
+      </c>
+      <c r="F84">
+        <v>6.4466670000000004E-2</v>
+      </c>
+    </row>
+    <row r="85" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A85" t="s">
+        <v>188</v>
+      </c>
+      <c r="B85" t="s">
+        <v>184</v>
+      </c>
+      <c r="D85" t="s">
+        <v>125</v>
+      </c>
+      <c r="E85" t="s">
+        <v>132</v>
+      </c>
+      <c r="F85">
+        <v>3.7258949999999999E-2</v>
+      </c>
+    </row>
+    <row r="86" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A86" t="s">
+        <v>188</v>
+      </c>
+      <c r="B86" t="s">
+        <v>184</v>
+      </c>
+      <c r="D86" t="s">
+        <v>127</v>
+      </c>
+      <c r="F86">
+        <v>37.258949999999999</v>
+      </c>
+    </row>
+    <row r="87" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A87" t="s">
+        <v>188</v>
+      </c>
+      <c r="B87" t="s">
+        <v>184</v>
+      </c>
+      <c r="D87" t="s">
+        <v>133</v>
+      </c>
+      <c r="F87">
+        <v>1.034971E-2</v>
+      </c>
+    </row>
+    <row r="88" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A88" t="s">
+        <v>188</v>
+      </c>
+      <c r="B88" t="s">
+        <v>184</v>
+      </c>
+      <c r="C88" t="s">
+        <v>134</v>
+      </c>
+      <c r="D88" t="s">
+        <v>125</v>
+      </c>
+      <c r="F88">
+        <v>4.1840000000000002</v>
+      </c>
+    </row>
+    <row r="89" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A89" t="s">
+        <v>188</v>
+      </c>
+      <c r="B89" t="s">
+        <v>184</v>
+      </c>
+      <c r="C89" t="s">
+        <v>135</v>
+      </c>
+      <c r="D89" t="s">
+        <v>127</v>
+      </c>
+      <c r="F89">
+        <v>0.35816920000000002</v>
+      </c>
+    </row>
+    <row r="90" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A90" t="s">
+        <v>188</v>
+      </c>
+      <c r="B90" t="s">
+        <v>185</v>
+      </c>
+      <c r="C90" t="s">
+        <v>134</v>
+      </c>
+      <c r="D90" t="s">
+        <v>127</v>
+      </c>
+      <c r="E90" t="s">
+        <v>136</v>
+      </c>
+      <c r="F90">
+        <v>4184</v>
+      </c>
+    </row>
+    <row r="91" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A91" t="s">
+        <v>188</v>
+      </c>
+      <c r="B91" t="str">
+        <f t="shared" ref="B91:B93" si="0">B90</f>
+        <v>Calorific value (volume basis-gases)</v>
+      </c>
+      <c r="C91" t="s">
+        <v>137</v>
+      </c>
+      <c r="D91" t="s">
+        <v>127</v>
+      </c>
+      <c r="E91" t="s">
+        <v>136</v>
+      </c>
+      <c r="F91">
+        <v>4.1840000000000002</v>
+      </c>
+    </row>
+    <row r="92" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A92" t="s">
+        <v>188</v>
+      </c>
+      <c r="B92" t="str">
+        <f t="shared" si="0"/>
+        <v>Calorific value (volume basis-gases)</v>
+      </c>
+      <c r="C92" t="s">
+        <v>131</v>
+      </c>
+      <c r="D92" t="s">
+        <v>127</v>
+      </c>
+      <c r="E92" t="s">
+        <v>136</v>
+      </c>
+      <c r="F92">
+        <v>37.258949999999999</v>
+      </c>
+    </row>
+    <row r="93" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A93" t="s">
+        <v>188</v>
+      </c>
+      <c r="B93" t="str">
+        <f t="shared" si="0"/>
+        <v>Calorific value (volume basis-gases)</v>
+      </c>
+      <c r="D93" t="s">
+        <v>128</v>
+      </c>
+      <c r="F93">
+        <v>1.034971E-2</v>
+      </c>
+    </row>
+    <row r="94" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A94" t="s">
+        <v>188</v>
+      </c>
+      <c r="B94" t="s">
+        <v>138</v>
+      </c>
+      <c r="C94" t="s">
+        <v>139</v>
+      </c>
+      <c r="D94" t="s">
+        <v>140</v>
+      </c>
+      <c r="E94" t="s">
+        <v>141</v>
+      </c>
+      <c r="F94">
+        <v>4.1867999999999999</v>
+      </c>
+    </row>
+    <row r="95" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A95" t="s">
+        <v>188</v>
+      </c>
+      <c r="B95" t="str">
+        <f t="shared" ref="B95:B96" si="1">B94</f>
+        <v>Specific entropy</v>
+      </c>
+      <c r="C95" t="s">
+        <v>142</v>
+      </c>
+      <c r="D95" t="s">
+        <v>143</v>
+      </c>
+      <c r="E95" t="s">
+        <v>141</v>
+      </c>
+      <c r="F95">
+        <v>4.1840000000000002</v>
+      </c>
+    </row>
+    <row r="96" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A96" t="s">
+        <v>188</v>
+      </c>
+      <c r="B96" t="str">
+        <f t="shared" si="1"/>
+        <v>Specific entropy</v>
+      </c>
+      <c r="C96" t="s">
+        <v>144</v>
+      </c>
+      <c r="D96" t="s">
+        <v>140</v>
+      </c>
+      <c r="E96" t="s">
+        <v>141</v>
+      </c>
+      <c r="F96">
+        <v>4.1840000000000002</v>
+      </c>
+    </row>
+    <row r="97" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A97" t="s">
+        <v>188</v>
+      </c>
+      <c r="B97" t="s">
+        <v>186</v>
+      </c>
+      <c r="C97" t="s">
+        <v>145</v>
+      </c>
+      <c r="D97" t="s">
+        <v>140</v>
+      </c>
+      <c r="E97" t="s">
+        <v>141</v>
+      </c>
+      <c r="F97">
+        <v>3600</v>
+      </c>
+    </row>
+    <row r="98" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A98" t="s">
+        <v>188</v>
+      </c>
+      <c r="B98" t="str">
+        <f t="shared" ref="B98:B99" si="2">B97</f>
+        <v>Specific-heat capacity (mass basis)</v>
+      </c>
+      <c r="C98" t="s">
+        <v>146</v>
+      </c>
+      <c r="D98" t="s">
+        <v>140</v>
+      </c>
+      <c r="E98" t="s">
+        <v>147</v>
+      </c>
+      <c r="F98">
+        <v>4.1867999999999999</v>
+      </c>
+    </row>
+    <row r="99" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A99" t="s">
+        <v>188</v>
+      </c>
+      <c r="B99" t="str">
+        <f t="shared" si="2"/>
+        <v>Specific-heat capacity (mass basis)</v>
+      </c>
+      <c r="C99" t="s">
+        <v>144</v>
+      </c>
+      <c r="D99" t="s">
+        <v>143</v>
+      </c>
+      <c r="E99" t="s">
+        <v>147</v>
+      </c>
+      <c r="F99">
+        <v>4.1840000000000002</v>
+      </c>
+    </row>
+    <row r="100" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A100" t="s">
+        <v>188</v>
+      </c>
+      <c r="B100" t="s">
+        <v>187</v>
+      </c>
+      <c r="C100" t="s">
+        <v>148</v>
+      </c>
+      <c r="D100" t="s">
+        <v>149</v>
+      </c>
+      <c r="F100">
+        <v>4.1867999999999999</v>
+      </c>
+    </row>
+    <row r="101" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A101" t="s">
+        <v>188</v>
+      </c>
+      <c r="B101" t="str">
+        <f t="shared" ref="B101" si="3">B100</f>
+        <v>Specific-heat capacity (mole basis)</v>
+      </c>
+      <c r="C101" t="s">
+        <v>150</v>
+      </c>
+      <c r="D101" t="s">
+        <v>149</v>
+      </c>
+      <c r="F101">
+        <v>4.1840000000000002</v>
+      </c>
+    </row>
+    <row r="102" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A102" t="s">
+        <v>151</v>
+      </c>
+      <c r="B102" t="s">
+        <v>152</v>
+      </c>
+      <c r="C102" t="s">
+        <v>153</v>
+      </c>
+      <c r="D102" t="s">
+        <v>154</v>
+      </c>
+      <c r="F102" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="103" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A103" t="s">
+        <v>151</v>
+      </c>
+      <c r="B103" t="str">
+        <f>B102</f>
+        <v>Temperature (absolute)</v>
+      </c>
+      <c r="C103" t="s">
+        <v>154</v>
+      </c>
+      <c r="D103" t="s">
+        <v>154</v>
+      </c>
+      <c r="F103">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="104" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A104" t="s">
+        <v>151</v>
+      </c>
+      <c r="B104" t="s">
+        <v>155</v>
+      </c>
+      <c r="C104" t="s">
+        <v>156</v>
+      </c>
+      <c r="D104" t="s">
+        <v>157</v>
+      </c>
+      <c r="F104" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="105" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A105" t="s">
+        <v>151</v>
+      </c>
+      <c r="B105" t="s">
+        <v>158</v>
+      </c>
+      <c r="C105" t="s">
+        <v>156</v>
+      </c>
+      <c r="D105" t="s">
+        <v>159</v>
+      </c>
+      <c r="F105" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="106" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A106" t="s">
+        <v>151</v>
+      </c>
+      <c r="B106" t="s">
+        <v>160</v>
+      </c>
+      <c r="C106" t="s">
+        <v>161</v>
+      </c>
+      <c r="D106" t="s">
+        <v>162</v>
+      </c>
+      <c r="F106">
+        <v>0.101325</v>
+      </c>
+    </row>
+    <row r="107" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A107" t="s">
+        <v>151</v>
+      </c>
+      <c r="B107" t="str">
+        <f t="shared" ref="B107:B121" si="4">B106</f>
+        <v>Pressure</v>
+      </c>
+      <c r="D107" t="s">
+        <v>163</v>
+      </c>
+      <c r="F107">
+        <v>101.325</v>
+      </c>
+    </row>
+    <row r="108" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A108" t="s">
+        <v>151</v>
+      </c>
+      <c r="B108" t="str">
+        <f t="shared" si="4"/>
+        <v>Pressure</v>
+      </c>
+      <c r="D108" t="s">
+        <v>164</v>
+      </c>
+      <c r="F108">
+        <v>1.01325</v>
+      </c>
+    </row>
+    <row r="109" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A109" t="s">
+        <v>151</v>
+      </c>
+      <c r="B109" t="str">
+        <f t="shared" si="4"/>
+        <v>Pressure</v>
+      </c>
+      <c r="C109" t="s">
+        <v>164</v>
+      </c>
+      <c r="D109" t="s">
+        <v>162</v>
+      </c>
+      <c r="F109">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="110" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A110" t="s">
+        <v>151</v>
+      </c>
+      <c r="B110" t="str">
+        <f t="shared" si="4"/>
+        <v>Pressure</v>
+      </c>
+      <c r="D110" t="s">
+        <v>163</v>
+      </c>
+      <c r="F110">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="111" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A111" t="s">
+        <v>151</v>
+      </c>
+      <c r="B111" t="str">
+        <f t="shared" si="4"/>
+        <v>Pressure</v>
+      </c>
+      <c r="C111" t="s">
+        <v>165</v>
+      </c>
+      <c r="D111" t="s">
+        <v>162</v>
+      </c>
+      <c r="F111">
+        <v>6.8947569999999996E-3</v>
+      </c>
+    </row>
+    <row r="112" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A112" t="s">
+        <v>151</v>
+      </c>
+      <c r="B112" t="str">
+        <f t="shared" si="4"/>
+        <v>Pressure</v>
+      </c>
+      <c r="D112" t="s">
+        <v>163</v>
+      </c>
+      <c r="F112">
+        <v>6.8947000000000003</v>
+      </c>
+    </row>
+    <row r="113" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A113" t="s">
+        <v>151</v>
+      </c>
+      <c r="B113" t="str">
+        <f t="shared" si="4"/>
+        <v>Pressure</v>
+      </c>
+      <c r="D113" t="s">
+        <v>164</v>
+      </c>
+      <c r="F113">
+        <v>6.894757E-2</v>
+      </c>
+    </row>
+    <row r="114" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A114" t="s">
+        <v>151</v>
+      </c>
+      <c r="B114" t="str">
+        <f t="shared" si="4"/>
+        <v>Pressure</v>
+      </c>
+      <c r="C114" t="s">
+        <v>166</v>
+      </c>
+      <c r="D114" t="s">
+        <v>163</v>
+      </c>
+      <c r="F114">
+        <v>3.3768500000000001</v>
+      </c>
+    </row>
+    <row r="115" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A115" t="s">
+        <v>151</v>
+      </c>
+      <c r="B115" t="str">
+        <f t="shared" si="4"/>
+        <v>Pressure</v>
+      </c>
+      <c r="C115" t="s">
+        <v>167</v>
+      </c>
+      <c r="D115" t="s">
+        <v>163</v>
+      </c>
+      <c r="F115">
+        <v>0.24884000000000001</v>
+      </c>
+    </row>
+    <row r="116" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A116" t="s">
+        <v>151</v>
+      </c>
+      <c r="B116" t="str">
+        <f t="shared" si="4"/>
+        <v>Pressure</v>
+      </c>
+      <c r="C116" t="s">
+        <v>168</v>
+      </c>
+      <c r="D116" t="s">
+        <v>163</v>
+      </c>
+      <c r="F116">
+        <v>0.13332240000000001</v>
+      </c>
+    </row>
+    <row r="117" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A117" t="s">
+        <v>151</v>
+      </c>
+      <c r="B117" t="str">
+        <f t="shared" si="4"/>
+        <v>Pressure</v>
+      </c>
+      <c r="C117" t="s">
+        <v>169</v>
+      </c>
+      <c r="D117" t="s">
+        <v>163</v>
+      </c>
+      <c r="F117">
+        <v>9.8063800000000007E-2</v>
+      </c>
+    </row>
+    <row r="118" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A118" t="s">
+        <v>151</v>
+      </c>
+      <c r="B118" t="str">
+        <f t="shared" si="4"/>
+        <v>Pressure</v>
+      </c>
+      <c r="C118" t="s">
+        <v>170</v>
+      </c>
+      <c r="D118" t="s">
+        <v>163</v>
+      </c>
+      <c r="F118">
+        <v>4.7880260000000001E-2</v>
+      </c>
+    </row>
+    <row r="119" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A119" t="s">
+        <v>151</v>
+      </c>
+      <c r="B119" t="str">
+        <f t="shared" si="4"/>
+        <v>Pressure</v>
+      </c>
+      <c r="C119" t="s">
+        <v>171</v>
+      </c>
+      <c r="D119" t="s">
+        <v>172</v>
+      </c>
+      <c r="F119">
+        <v>0.13332240000000001</v>
+      </c>
+    </row>
+    <row r="120" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A120" t="s">
+        <v>151</v>
+      </c>
+      <c r="B120" t="str">
+        <f t="shared" si="4"/>
+        <v>Pressure</v>
+      </c>
+      <c r="C120" t="s">
+        <v>164</v>
+      </c>
+      <c r="D120" t="s">
+        <v>172</v>
+      </c>
+      <c r="F120">
+        <v>100000</v>
+      </c>
+    </row>
+    <row r="121" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A121" t="s">
+        <v>151</v>
+      </c>
+      <c r="B121" t="str">
+        <f t="shared" si="4"/>
+        <v>Pressure</v>
+      </c>
+      <c r="C121" t="s">
+        <v>173</v>
+      </c>
+      <c r="D121" t="s">
+        <v>172</v>
+      </c>
+      <c r="F121">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="122" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A122" t="s">
+        <v>151</v>
+      </c>
+      <c r="B122" t="s">
+        <v>174</v>
+      </c>
+      <c r="C122" t="s">
+        <v>175</v>
+      </c>
+      <c r="D122" t="s">
+        <v>163</v>
+      </c>
+      <c r="F122">
+        <v>3.3768500000000001</v>
+      </c>
+    </row>
+    <row r="123" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A123" t="s">
+        <v>151</v>
+      </c>
+      <c r="B123" t="str">
+        <f t="shared" ref="B123:B126" si="5">B122</f>
+        <v>Vacuum, draft</v>
+      </c>
+      <c r="C123" t="s">
+        <v>176</v>
+      </c>
+      <c r="D123" t="s">
+        <v>163</v>
+      </c>
+      <c r="F123">
+        <v>0.249082</v>
+      </c>
+    </row>
+    <row r="124" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A124" t="s">
+        <v>151</v>
+      </c>
+      <c r="B124" t="str">
+        <f t="shared" si="5"/>
+        <v>Vacuum, draft</v>
+      </c>
+      <c r="C124" t="s">
+        <v>177</v>
+      </c>
+      <c r="D124" t="s">
+        <v>163</v>
+      </c>
+      <c r="F124">
+        <v>0.24884000000000001</v>
+      </c>
+    </row>
+    <row r="125" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A125" t="s">
+        <v>151</v>
+      </c>
+      <c r="B125" t="str">
+        <f t="shared" si="5"/>
+        <v>Vacuum, draft</v>
+      </c>
+      <c r="C125" t="s">
+        <v>165</v>
+      </c>
+      <c r="D125" t="s">
+        <v>163</v>
+      </c>
+      <c r="F125">
+        <v>0.13332240000000001</v>
+      </c>
+    </row>
+    <row r="126" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A126" t="s">
+        <v>151</v>
+      </c>
+      <c r="B126" t="str">
+        <f t="shared" si="5"/>
+        <v>Vacuum, draft</v>
+      </c>
+      <c r="C126" t="s">
+        <v>169</v>
+      </c>
+      <c r="D126" t="s">
+        <v>163</v>
+      </c>
+      <c r="F126">
+        <v>9.8062999999999997E-2</v>
+      </c>
+    </row>
+    <row r="127" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A127" t="s">
+        <v>151</v>
+      </c>
+      <c r="B127" t="s">
+        <v>178</v>
+      </c>
+      <c r="C127" t="s">
+        <v>8</v>
+      </c>
+      <c r="D127" t="s">
+        <v>4</v>
+      </c>
+      <c r="F127">
+        <v>0.30480000000000002</v>
+      </c>
+    </row>
+    <row r="128" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A128" t="s">
+        <v>151</v>
+      </c>
+      <c r="B128" t="str">
+        <f t="shared" ref="B128:B129" si="6">B127</f>
+        <v>Liquid head</v>
+      </c>
+      <c r="C128" t="s">
+        <v>10</v>
+      </c>
+      <c r="D128" t="s">
+        <v>11</v>
+      </c>
+      <c r="F128">
+        <v>25.4</v>
+      </c>
+    </row>
+    <row r="129" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A129" t="s">
+        <v>151</v>
+      </c>
+      <c r="B129" t="str">
+        <f t="shared" si="6"/>
+        <v>Liquid head</v>
+      </c>
+      <c r="D129" t="s">
+        <v>9</v>
+      </c>
+      <c r="F129">
+        <v>2.54</v>
+      </c>
+    </row>
+    <row r="130" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A130" t="s">
+        <v>151</v>
+      </c>
+      <c r="B130" t="s">
+        <v>179</v>
+      </c>
+      <c r="C130" t="s">
+        <v>180</v>
+      </c>
+      <c r="D130" t="s">
+        <v>181</v>
+      </c>
+      <c r="F130">
+        <v>22.62059</v>
+      </c>
+    </row>
+    <row r="131" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A131" s="1" t="s">
+        <v>285</v>
+      </c>
+      <c r="B131" s="1" t="s">
+        <v>193</v>
+      </c>
+      <c r="C131" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="D131" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="E131" s="1"/>
+      <c r="F131" s="1">
+        <v>16.018460000000001</v>
+      </c>
+      <c r="G131" s="1" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="132" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A132" t="str">
+        <f t="shared" ref="A132:A163" si="7">A131</f>
+        <v>Density, specific volume, concentration, dosage</v>
+      </c>
+      <c r="B132" t="str">
+        <f t="shared" ref="B132:B139" si="8">B131</f>
+        <v>Density</v>
+      </c>
+      <c r="C132" t="str">
+        <f>C131</f>
+        <v>lbm/ft</v>
+      </c>
+      <c r="D132" t="s">
+        <v>196</v>
+      </c>
+      <c r="F132">
+        <v>16018.46</v>
+      </c>
+    </row>
+    <row r="133" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A133" t="str">
+        <f t="shared" si="7"/>
+        <v>Density, specific volume, concentration, dosage</v>
+      </c>
+      <c r="B133" t="str">
+        <f t="shared" si="8"/>
+        <v>Density</v>
+      </c>
+      <c r="C133" t="s">
+        <v>197</v>
+      </c>
+      <c r="D133" t="s">
+        <v>195</v>
+      </c>
+      <c r="F133">
+        <v>119.82640000000001</v>
+      </c>
+    </row>
+    <row r="134" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A134" t="str">
+        <f t="shared" si="7"/>
+        <v>Density, specific volume, concentration, dosage</v>
+      </c>
+      <c r="B134" t="str">
+        <f t="shared" si="8"/>
+        <v>Density</v>
+      </c>
+      <c r="C134" t="str">
+        <f>C133</f>
+        <v>lbm/U.S. gal</v>
+      </c>
+      <c r="D134" t="s">
+        <v>198</v>
+      </c>
+      <c r="F134">
+        <v>0.1198264</v>
+      </c>
+    </row>
+    <row r="135" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A135" t="str">
+        <f t="shared" si="7"/>
+        <v>Density, specific volume, concentration, dosage</v>
+      </c>
+      <c r="B135" t="str">
+        <f t="shared" si="8"/>
+        <v>Density</v>
+      </c>
+      <c r="C135" t="s">
+        <v>199</v>
+      </c>
+      <c r="D135" t="s">
+        <v>195</v>
+      </c>
+      <c r="F135">
+        <v>99.776300000000006</v>
+      </c>
+    </row>
+    <row r="136" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A136" t="str">
+        <f t="shared" si="7"/>
+        <v>Density, specific volume, concentration, dosage</v>
+      </c>
+      <c r="B136" t="str">
+        <f t="shared" si="8"/>
+        <v>Density</v>
+      </c>
+      <c r="C136" t="s">
+        <v>200</v>
+      </c>
+      <c r="D136" t="s">
+        <v>195</v>
+      </c>
+      <c r="F136">
+        <v>16.018460000000001</v>
+      </c>
+    </row>
+    <row r="137" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A137" t="str">
+        <f t="shared" si="7"/>
+        <v>Density, specific volume, concentration, dosage</v>
+      </c>
+      <c r="B137" t="str">
+        <f t="shared" si="8"/>
+        <v>Density</v>
+      </c>
+      <c r="C137" t="str">
+        <f>C136</f>
+        <v>lbm/ft3</v>
+      </c>
+      <c r="D137" t="s">
+        <v>198</v>
+      </c>
+      <c r="F137">
+        <v>1.6018460000000002E-2</v>
+      </c>
+    </row>
+    <row r="138" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A138" t="str">
+        <f t="shared" si="7"/>
+        <v>Density, specific volume, concentration, dosage</v>
+      </c>
+      <c r="B138" t="str">
+        <f t="shared" si="8"/>
+        <v>Density</v>
+      </c>
+      <c r="C138" t="s">
+        <v>198</v>
+      </c>
+      <c r="D138" t="s">
+        <v>195</v>
+      </c>
+      <c r="F138">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="139" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A139" t="str">
+        <f t="shared" si="7"/>
+        <v>Density, specific volume, concentration, dosage</v>
+      </c>
+      <c r="B139" t="str">
+        <f t="shared" si="8"/>
+        <v>Density</v>
+      </c>
+      <c r="C139" t="s">
+        <v>200</v>
+      </c>
+      <c r="D139" t="s">
+        <v>195</v>
+      </c>
+      <c r="F139">
+        <v>16.018460000000001</v>
+      </c>
+    </row>
+    <row r="140" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A140" t="str">
+        <f t="shared" si="7"/>
+        <v>Density, specific volume, concentration, dosage</v>
+      </c>
+      <c r="B140" t="s">
+        <v>201</v>
+      </c>
+      <c r="C140" t="s">
+        <v>202</v>
+      </c>
+      <c r="D140" t="s">
+        <v>203</v>
+      </c>
+      <c r="F140">
+        <v>6.2427959999999998E-2</v>
+      </c>
+    </row>
+    <row r="141" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A141" t="str">
+        <f t="shared" si="7"/>
+        <v>Density, specific volume, concentration, dosage</v>
+      </c>
+      <c r="B141" t="str">
+        <f t="shared" ref="B141:B144" si="9">B140</f>
+        <v>Specific volume</v>
+      </c>
+      <c r="C141" t="str">
+        <f>C140</f>
+        <v>ft3/lbm</v>
+      </c>
+      <c r="D141" t="s">
+        <v>204</v>
+      </c>
+      <c r="F141">
+        <v>6.2427960000000003E-5</v>
+      </c>
+    </row>
+    <row r="142" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A142" t="str">
+        <f t="shared" si="7"/>
+        <v>Density, specific volume, concentration, dosage</v>
+      </c>
+      <c r="B142" t="str">
+        <f t="shared" si="9"/>
+        <v>Specific volume</v>
+      </c>
+      <c r="C142" t="s">
+        <v>202</v>
+      </c>
+      <c r="D142" t="s">
+        <v>205</v>
+      </c>
+      <c r="F142">
+        <v>62.427900000000001</v>
+      </c>
+    </row>
+    <row r="143" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A143" t="str">
+        <f t="shared" si="7"/>
+        <v>Density, specific volume, concentration, dosage</v>
+      </c>
+      <c r="B143" t="str">
+        <f t="shared" si="9"/>
+        <v>Specific volume</v>
+      </c>
+      <c r="C143" t="s">
+        <v>206</v>
+      </c>
+      <c r="D143" t="s">
+        <v>205</v>
+      </c>
+      <c r="E143" t="s">
+        <v>207</v>
+      </c>
+      <c r="F143">
+        <v>10.02242</v>
+      </c>
+    </row>
+    <row r="144" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A144" t="str">
+        <f t="shared" si="7"/>
+        <v>Density, specific volume, concentration, dosage</v>
+      </c>
+      <c r="B144" t="str">
+        <f t="shared" si="9"/>
+        <v>Specific volume</v>
+      </c>
+      <c r="C144" t="s">
+        <v>208</v>
+      </c>
+      <c r="D144" t="s">
+        <v>205</v>
+      </c>
+      <c r="E144" t="s">
+        <v>207</v>
+      </c>
+      <c r="F144">
+        <v>8.3454040000000003</v>
+      </c>
+    </row>
+    <row r="145" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A145" t="str">
+        <f t="shared" si="7"/>
+        <v>Density, specific volume, concentration, dosage</v>
+      </c>
+      <c r="B145" t="s">
+        <v>209</v>
+      </c>
+      <c r="C145" t="s">
+        <v>210</v>
+      </c>
+      <c r="D145" t="s">
+        <v>211</v>
+      </c>
+      <c r="F145">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="146" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A146" t="str">
+        <f t="shared" si="7"/>
+        <v>Density, specific volume, concentration, dosage</v>
+      </c>
+      <c r="B146" t="str">
+        <f>B145</f>
+        <v>Specific volume (mole basis)</v>
+      </c>
+      <c r="C146" t="s">
+        <v>212</v>
+      </c>
+      <c r="D146" t="s">
+        <v>211</v>
+      </c>
+      <c r="F146">
+        <v>6.2427959999999998E-2</v>
+      </c>
+    </row>
+    <row r="147" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A147" t="str">
+        <f t="shared" si="7"/>
+        <v>Density, specific volume, concentration, dosage</v>
+      </c>
+      <c r="B147" t="s">
+        <v>201</v>
+      </c>
+      <c r="C147" t="s">
+        <v>213</v>
+      </c>
+      <c r="D147" t="s">
+        <v>214</v>
+      </c>
+      <c r="F147">
+        <v>0.17525350000000001</v>
+      </c>
+    </row>
+    <row r="148" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A148" t="str">
+        <f t="shared" si="7"/>
+        <v>Density, specific volume, concentration, dosage</v>
+      </c>
+      <c r="B148" t="str">
+        <f>B147</f>
+        <v>Specific volume</v>
+      </c>
+      <c r="C148" t="s">
+        <v>215</v>
+      </c>
+      <c r="D148" t="s">
+        <v>214</v>
+      </c>
+      <c r="F148">
+        <v>0.15647630000000001</v>
+      </c>
+    </row>
+    <row r="149" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A149" t="str">
+        <f t="shared" si="7"/>
+        <v>Density, specific volume, concentration, dosage</v>
+      </c>
+      <c r="B149" t="s">
+        <v>216</v>
+      </c>
+      <c r="C149" t="s">
+        <v>213</v>
+      </c>
+      <c r="D149" t="s">
+        <v>217</v>
+      </c>
+      <c r="E149" t="s">
+        <v>218</v>
+      </c>
+      <c r="F149">
+        <v>175.2535</v>
+      </c>
+    </row>
+    <row r="150" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A150" t="str">
+        <f t="shared" si="7"/>
+        <v>Density, specific volume, concentration, dosage</v>
+      </c>
+      <c r="B150" t="str">
+        <f t="shared" ref="B150:B152" si="10">B149</f>
+        <v>Yield</v>
+      </c>
+      <c r="C150" t="s">
+        <v>215</v>
+      </c>
+      <c r="D150" t="s">
+        <v>217</v>
+      </c>
+      <c r="E150" t="s">
+        <v>218</v>
+      </c>
+      <c r="F150">
+        <v>156.47630000000001</v>
+      </c>
+    </row>
+    <row r="151" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A151" t="str">
+        <f t="shared" si="7"/>
+        <v>Density, specific volume, concentration, dosage</v>
+      </c>
+      <c r="B151" t="str">
+        <f t="shared" si="10"/>
+        <v>Yield</v>
+      </c>
+      <c r="C151" t="s">
+        <v>219</v>
+      </c>
+      <c r="D151" t="s">
+        <v>220</v>
+      </c>
+      <c r="E151" t="s">
+        <v>218</v>
+      </c>
+      <c r="F151">
+        <v>4.1727020000000001</v>
+      </c>
+    </row>
+    <row r="152" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A152" t="str">
+        <f t="shared" si="7"/>
+        <v>Density, specific volume, concentration, dosage</v>
+      </c>
+      <c r="B152" t="str">
+        <f t="shared" si="10"/>
+        <v>Yield</v>
+      </c>
+      <c r="C152" t="s">
+        <v>221</v>
+      </c>
+      <c r="D152" t="s">
+        <v>217</v>
+      </c>
+      <c r="E152" t="s">
+        <v>218</v>
+      </c>
+      <c r="F152">
+        <v>3.7256269999999998</v>
+      </c>
+    </row>
+    <row r="153" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A153" t="str">
+        <f t="shared" si="7"/>
+        <v>Density, specific volume, concentration, dosage</v>
+      </c>
+      <c r="B153" t="s">
+        <v>222</v>
+      </c>
+      <c r="C153" t="s">
+        <v>223</v>
+      </c>
+      <c r="D153" t="s">
+        <v>224</v>
+      </c>
+      <c r="F153">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="154" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A154" t="str">
+        <f t="shared" si="7"/>
+        <v>Density, specific volume, concentration, dosage</v>
+      </c>
+      <c r="B154" t="str">
+        <f t="shared" ref="B154:B155" si="11">B153</f>
+        <v>Concentration (mass/mass)</v>
+      </c>
+      <c r="C154" t="str">
+        <f>C153</f>
+        <v>wt %</v>
+      </c>
+      <c r="D154" t="s">
+        <v>225</v>
+      </c>
+      <c r="F154">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="155" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A155" t="str">
+        <f t="shared" si="7"/>
+        <v>Density, specific volume, concentration, dosage</v>
+      </c>
+      <c r="B155" t="str">
+        <f t="shared" si="11"/>
+        <v>Concentration (mass/mass)</v>
+      </c>
+      <c r="C155" t="s">
+        <v>226</v>
+      </c>
+      <c r="D155" t="s">
+        <v>227</v>
+      </c>
+      <c r="F155">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="156" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A156" t="str">
+        <f t="shared" si="7"/>
+        <v>Density, specific volume, concentration, dosage</v>
+      </c>
+      <c r="B156" t="s">
+        <v>228</v>
+      </c>
+      <c r="C156" t="s">
+        <v>229</v>
+      </c>
+      <c r="D156" t="s">
+        <v>195</v>
+      </c>
+      <c r="E156" t="s">
+        <v>230</v>
+      </c>
+      <c r="F156">
+        <v>2.8530099999999998</v>
+      </c>
+    </row>
+    <row r="157" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A157" t="str">
+        <f t="shared" si="7"/>
+        <v>Density, specific volume, concentration, dosage</v>
+      </c>
+      <c r="B157" t="str">
+        <f t="shared" ref="B157:B165" si="12">B156</f>
+        <v>Concentration (mass/volume)</v>
+      </c>
+      <c r="C157" t="s">
+        <v>231</v>
+      </c>
+      <c r="D157" t="s">
+        <v>195</v>
+      </c>
+      <c r="F157">
+        <v>0.26417200000000002</v>
+      </c>
+    </row>
+    <row r="158" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A158" t="str">
+        <f t="shared" si="7"/>
+        <v>Density, specific volume, concentration, dosage</v>
+      </c>
+      <c r="B158" t="str">
+        <f t="shared" si="12"/>
+        <v>Concentration (mass/volume)</v>
+      </c>
+      <c r="C158" t="s">
+        <v>232</v>
+      </c>
+      <c r="D158" t="s">
+        <v>195</v>
+      </c>
+      <c r="E158" t="s">
+        <v>233</v>
+      </c>
+      <c r="F158">
+        <v>0.219969</v>
+      </c>
+    </row>
+    <row r="159" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A159" t="str">
+        <f t="shared" si="7"/>
+        <v>Density, specific volume, concentration, dosage</v>
+      </c>
+      <c r="B159" t="str">
+        <f t="shared" si="12"/>
+        <v>Concentration (mass/volume)</v>
+      </c>
+      <c r="C159" t="s">
+        <v>234</v>
+      </c>
+      <c r="D159" t="s">
+        <v>235</v>
+      </c>
+      <c r="E159" t="s">
+        <v>236</v>
+      </c>
+      <c r="F159">
+        <v>119.82640000000001</v>
+      </c>
+    </row>
+    <row r="160" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A160" t="str">
+        <f t="shared" si="7"/>
+        <v>Density, specific volume, concentration, dosage</v>
+      </c>
+      <c r="B160" t="str">
+        <f t="shared" si="12"/>
+        <v>Concentration (mass/volume)</v>
+      </c>
+      <c r="C160" t="s">
+        <v>237</v>
+      </c>
+      <c r="D160" t="s">
+        <v>196</v>
+      </c>
+      <c r="E160" t="s">
+        <v>236</v>
+      </c>
+      <c r="F160">
+        <v>99.776300000000006</v>
+      </c>
+    </row>
+    <row r="161" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A161" t="str">
+        <f t="shared" si="7"/>
+        <v>Density, specific volume, concentration, dosage</v>
+      </c>
+      <c r="B161" t="str">
+        <f t="shared" si="12"/>
+        <v>Concentration (mass/volume)</v>
+      </c>
+      <c r="C161" t="s">
+        <v>238</v>
+      </c>
+      <c r="D161" t="s">
+        <v>196</v>
+      </c>
+      <c r="E161" t="s">
+        <v>236</v>
+      </c>
+      <c r="F161">
+        <v>17.11806</v>
+      </c>
+    </row>
+    <row r="162" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A162" t="str">
+        <f t="shared" si="7"/>
+        <v>Density, specific volume, concentration, dosage</v>
+      </c>
+      <c r="B162" t="str">
+        <f t="shared" si="12"/>
+        <v>Concentration (mass/volume)</v>
+      </c>
+      <c r="C162" t="s">
+        <v>239</v>
+      </c>
+      <c r="D162" t="s">
+        <v>240</v>
+      </c>
+      <c r="F162">
+        <v>2288.3510000000001</v>
+      </c>
+    </row>
+    <row r="163" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A163" t="str">
+        <f t="shared" si="7"/>
+        <v>Density, specific volume, concentration, dosage</v>
+      </c>
+      <c r="B163" t="str">
+        <f t="shared" si="12"/>
+        <v>Concentration (mass/volume)</v>
+      </c>
+      <c r="C163" t="s">
+        <v>241</v>
+      </c>
+      <c r="D163" t="s">
+        <v>196</v>
+      </c>
+      <c r="E163" t="s">
+        <v>236</v>
+      </c>
+      <c r="F163">
+        <v>2.8530099999999998</v>
+      </c>
+    </row>
+    <row r="164" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A164" t="str">
+        <f t="shared" ref="A164:A182" si="13">A163</f>
+        <v>Density, specific volume, concentration, dosage</v>
+      </c>
+      <c r="B164" t="str">
+        <f t="shared" si="12"/>
+        <v>Concentration (mass/volume)</v>
+      </c>
+      <c r="C164" t="s">
+        <v>242</v>
+      </c>
+      <c r="D164" t="s">
+        <v>196</v>
+      </c>
+      <c r="E164" t="s">
+        <v>236</v>
+      </c>
+      <c r="F164">
+        <v>0.26417200000000002</v>
+      </c>
+    </row>
+    <row r="165" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A165" t="str">
+        <f t="shared" si="13"/>
+        <v>Density, specific volume, concentration, dosage</v>
+      </c>
+      <c r="B165" t="str">
+        <f t="shared" si="12"/>
+        <v>Concentration (mass/volume)</v>
+      </c>
+      <c r="C165" t="s">
+        <v>243</v>
+      </c>
+      <c r="D165" t="s">
+        <v>240</v>
+      </c>
+      <c r="F165">
+        <v>22.883510000000001</v>
+      </c>
+    </row>
+    <row r="166" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A166" t="str">
+        <f t="shared" si="13"/>
+        <v>Density, specific volume, concentration, dosage</v>
+      </c>
+      <c r="B166" t="s">
+        <v>244</v>
+      </c>
+      <c r="C166" t="s">
+        <v>245</v>
+      </c>
+      <c r="D166" t="s">
+        <v>246</v>
+      </c>
+      <c r="F166">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="167" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A167" t="str">
+        <f t="shared" si="13"/>
+        <v>Density, specific volume, concentration, dosage</v>
+      </c>
+      <c r="B167" t="str">
+        <f t="shared" ref="B167:B177" si="14">B166</f>
+        <v>Concentration (volume/volume)</v>
+      </c>
+      <c r="C167" t="s">
+        <v>247</v>
+      </c>
+      <c r="D167" t="s">
+        <v>248</v>
+      </c>
+      <c r="F167">
+        <v>1.2889309999999999E-4</v>
+      </c>
+    </row>
+    <row r="168" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A168" t="str">
+        <f t="shared" si="13"/>
+        <v>Density, specific volume, concentration, dosage</v>
+      </c>
+      <c r="B168" t="str">
+        <f t="shared" si="14"/>
+        <v>Concentration (volume/volume)</v>
+      </c>
+      <c r="C168" t="s">
+        <v>249</v>
+      </c>
+      <c r="D168" t="s">
+        <v>248</v>
+      </c>
+      <c r="F168">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="169" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A169" t="str">
+        <f t="shared" si="13"/>
+        <v>Density, specific volume, concentration, dosage</v>
+      </c>
+      <c r="B169" t="str">
+        <f t="shared" si="14"/>
+        <v>Concentration (volume/volume)</v>
+      </c>
+      <c r="C169" t="s">
+        <v>250</v>
+      </c>
+      <c r="D169" t="s">
+        <v>251</v>
+      </c>
+      <c r="E169" t="s">
+        <v>252</v>
+      </c>
+      <c r="F169">
+        <v>160.5437</v>
+      </c>
+    </row>
+    <row r="170" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A170" t="str">
+        <f t="shared" si="13"/>
+        <v>Density, specific volume, concentration, dosage</v>
+      </c>
+      <c r="B170" t="str">
+        <f t="shared" si="14"/>
+        <v>Concentration (volume/volume)</v>
+      </c>
+      <c r="C170" t="s">
+        <v>253</v>
+      </c>
+      <c r="D170" t="s">
+        <v>251</v>
+      </c>
+      <c r="E170" t="s">
+        <v>252</v>
+      </c>
+      <c r="F170">
+        <v>1.3368059999999999E-2</v>
+      </c>
+    </row>
+    <row r="171" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A171" t="str">
+        <f t="shared" si="13"/>
+        <v>Density, specific volume, concentration, dosage</v>
+      </c>
+      <c r="B171" t="str">
+        <f t="shared" si="14"/>
+        <v>Concentration (volume/volume)</v>
+      </c>
+      <c r="C171" t="s">
+        <v>254</v>
+      </c>
+      <c r="D171" t="s">
+        <v>251</v>
+      </c>
+      <c r="E171" t="s">
+        <v>252</v>
+      </c>
+      <c r="F171">
+        <v>0.26417200000000002</v>
+      </c>
+    </row>
+    <row r="172" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A172" t="str">
+        <f t="shared" si="13"/>
+        <v>Density, specific volume, concentration, dosage</v>
+      </c>
+      <c r="B172" t="str">
+        <f t="shared" si="14"/>
+        <v>Concentration (volume/volume)</v>
+      </c>
+      <c r="C172" t="s">
+        <v>255</v>
+      </c>
+      <c r="D172" t="s">
+        <v>251</v>
+      </c>
+      <c r="E172" t="s">
+        <v>252</v>
+      </c>
+      <c r="F172">
+        <v>0.2199692</v>
+      </c>
+    </row>
+    <row r="173" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A173" t="str">
+        <f t="shared" si="13"/>
+        <v>Density, specific volume, concentration, dosage</v>
+      </c>
+      <c r="B173" t="str">
+        <f t="shared" si="14"/>
+        <v>Concentration (volume/volume)</v>
+      </c>
+      <c r="C173" t="s">
+        <v>256</v>
+      </c>
+      <c r="D173" t="s">
+        <v>257</v>
+      </c>
+      <c r="F173">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="174" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A174" t="str">
+        <f t="shared" si="13"/>
+        <v>Density, specific volume, concentration, dosage</v>
+      </c>
+      <c r="B174" t="str">
+        <f t="shared" si="14"/>
+        <v>Concentration (volume/volume)</v>
+      </c>
+      <c r="C174" t="str">
+        <f>C173</f>
+        <v>vol ppm</v>
+      </c>
+      <c r="D174" t="s">
+        <v>251</v>
+      </c>
+      <c r="E174" t="s">
+        <v>252</v>
+      </c>
+      <c r="F174">
+        <v>1E-3</v>
+      </c>
+    </row>
+    <row r="175" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A175" t="str">
+        <f t="shared" si="13"/>
+        <v>Density, specific volume, concentration, dosage</v>
+      </c>
+      <c r="B175" t="str">
+        <f t="shared" si="14"/>
+        <v>Concentration (volume/volume)</v>
+      </c>
+      <c r="C175" t="s">
+        <v>258</v>
+      </c>
+      <c r="D175" t="s">
+        <v>257</v>
+      </c>
+      <c r="F175">
+        <v>28.59403</v>
+      </c>
+    </row>
+    <row r="176" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A176" t="str">
+        <f t="shared" si="13"/>
+        <v>Density, specific volume, concentration, dosage</v>
+      </c>
+      <c r="B176" t="str">
+        <f t="shared" si="14"/>
+        <v>Concentration (volume/volume)</v>
+      </c>
+      <c r="C176" t="s">
+        <v>259</v>
+      </c>
+      <c r="D176" t="s">
+        <v>257</v>
+      </c>
+      <c r="F176">
+        <v>23.809000000000001</v>
+      </c>
+    </row>
+    <row r="177" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A177" t="str">
+        <f t="shared" si="13"/>
+        <v>Density, specific volume, concentration, dosage</v>
+      </c>
+      <c r="B177" t="str">
+        <f t="shared" si="14"/>
+        <v>Concentration (volume/volume)</v>
+      </c>
+      <c r="C177" t="s">
+        <v>260</v>
+      </c>
+      <c r="D177" t="s">
+        <v>257</v>
+      </c>
+      <c r="F177">
+        <v>3.5742530000000001</v>
+      </c>
+    </row>
+    <row r="178" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A178" t="str">
+        <f t="shared" si="13"/>
+        <v>Density, specific volume, concentration, dosage</v>
+      </c>
+      <c r="B178" t="s">
+        <v>261</v>
+      </c>
+      <c r="C178" t="s">
+        <v>262</v>
+      </c>
+      <c r="D178" t="s">
+        <v>263</v>
+      </c>
+      <c r="F178">
+        <v>119.82640000000001</v>
+      </c>
+    </row>
+    <row r="179" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A179" t="str">
+        <f t="shared" si="13"/>
+        <v>Density, specific volume, concentration, dosage</v>
+      </c>
+      <c r="B179" t="str">
+        <f t="shared" ref="B179:B181" si="15">B178</f>
+        <v>Concentration (mole/volume)</v>
+      </c>
+      <c r="C179" t="s">
+        <v>264</v>
+      </c>
+      <c r="D179" t="s">
+        <v>263</v>
+      </c>
+      <c r="F179">
+        <v>99.776439999999994</v>
+      </c>
+    </row>
+    <row r="180" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A180" t="str">
+        <f t="shared" si="13"/>
+        <v>Density, specific volume, concentration, dosage</v>
+      </c>
+      <c r="B180" t="str">
+        <f t="shared" si="15"/>
+        <v>Concentration (mole/volume)</v>
+      </c>
+      <c r="C180" t="s">
+        <v>265</v>
+      </c>
+      <c r="D180" t="s">
+        <v>263</v>
+      </c>
+      <c r="F180">
+        <v>16.018460000000001</v>
+      </c>
+    </row>
+    <row r="181" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A181" t="str">
+        <f t="shared" si="13"/>
+        <v>Density, specific volume, concentration, dosage</v>
+      </c>
+      <c r="B181" t="str">
+        <f t="shared" si="15"/>
+        <v>Concentration (mole/volume)</v>
+      </c>
+      <c r="C181" t="s">
+        <v>266</v>
+      </c>
+      <c r="D181" t="s">
+        <v>263</v>
+      </c>
+      <c r="F181">
+        <v>7.51821E-3</v>
+      </c>
+    </row>
+    <row r="182" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A182" t="str">
+        <f t="shared" si="13"/>
+        <v>Density, specific volume, concentration, dosage</v>
+      </c>
+      <c r="B182" t="s">
+        <v>267</v>
+      </c>
+      <c r="C182" t="s">
+        <v>268</v>
+      </c>
+      <c r="D182" t="s">
+        <v>269</v>
+      </c>
+      <c r="E182" t="s">
+        <v>270</v>
+      </c>
+      <c r="F182">
+        <v>3.1669</v>
+      </c>
+    </row>
+    <row r="183" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A183" t="str">
+        <f t="shared" ref="A183:B183" si="16">A182</f>
+        <v>Density, specific volume, concentration, dosage</v>
+      </c>
+      <c r="B183" t="str">
+        <f t="shared" si="16"/>
+        <v>Concentration (volume/mole)</v>
+      </c>
+      <c r="C183" t="s">
+        <v>271</v>
+      </c>
+      <c r="D183" t="s">
+        <v>269</v>
+      </c>
+      <c r="E183" t="s">
+        <v>270</v>
+      </c>
+      <c r="F183">
+        <v>0.13300999999999999</v>
+      </c>
+    </row>
+    <row r="184" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A184" t="s">
+        <v>272</v>
+      </c>
+      <c r="B184" t="s">
+        <v>273</v>
+      </c>
+      <c r="C184" t="s">
+        <v>274</v>
+      </c>
+      <c r="D184" t="s">
+        <v>275</v>
+      </c>
+      <c r="F184">
+        <v>1.0160469999999999</v>
+      </c>
+    </row>
+    <row r="185" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A185" t="str">
+        <f t="shared" ref="A185:B186" si="17">A184</f>
+        <v>Facility throughput, capacity</v>
+      </c>
+      <c r="B185" t="str">
+        <f t="shared" si="17"/>
+        <v>Throughput (mass basis)</v>
+      </c>
+      <c r="C185" t="s">
+        <v>276</v>
+      </c>
+      <c r="D185" t="s">
+        <v>275</v>
+      </c>
+      <c r="F185">
+        <v>0.90718469999999996</v>
+      </c>
+    </row>
+    <row r="186" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A186" t="str">
+        <f t="shared" si="17"/>
+        <v>Facility throughput, capacity</v>
+      </c>
+      <c r="B186" t="str">
+        <f t="shared" si="17"/>
+        <v>Throughput (mass basis)</v>
+      </c>
+      <c r="C186" t="s">
+        <v>277</v>
+      </c>
+      <c r="D186" t="s">
+        <v>278</v>
+      </c>
+      <c r="F186">
+        <v>1.0160469999999999</v>
+      </c>
+    </row>
+    <row r="187" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A187" t="str">
+        <f t="shared" ref="A187:C187" si="18">A186</f>
+        <v>Facility throughput, capacity</v>
+      </c>
+      <c r="B187" t="str">
+        <f t="shared" si="18"/>
+        <v>Throughput (mass basis)</v>
+      </c>
+      <c r="C187" t="str">
+        <f t="shared" si="18"/>
+        <v>U.K. ton/day</v>
+      </c>
+      <c r="D187" t="s">
+        <v>279</v>
+      </c>
+      <c r="F187">
+        <v>4.2335289999999998E-2</v>
+      </c>
+    </row>
+    <row r="188" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A188" t="str">
+        <f t="shared" ref="A188:B188" si="19">A187</f>
+        <v>Facility throughput, capacity</v>
+      </c>
+      <c r="B188" t="str">
+        <f t="shared" si="19"/>
+        <v>Throughput (mass basis)</v>
+      </c>
+      <c r="C188" t="s">
+        <v>280</v>
+      </c>
+      <c r="D188" t="s">
+        <v>278</v>
+      </c>
+      <c r="F188">
+        <v>0.90718469999999996</v>
+      </c>
+    </row>
+    <row r="189" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A189" t="str">
+        <f t="shared" ref="A189:C189" si="20">A188</f>
+        <v>Facility throughput, capacity</v>
+      </c>
+      <c r="B189" t="str">
+        <f t="shared" si="20"/>
+        <v>Throughput (mass basis)</v>
+      </c>
+      <c r="C189" t="str">
+        <f t="shared" si="20"/>
+        <v>U.S. ton/day</v>
+      </c>
+      <c r="D189" t="s">
+        <v>279</v>
+      </c>
+      <c r="F189">
+        <v>3.7799359999999997E-2</v>
+      </c>
+    </row>
+    <row r="190" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A190" t="str">
+        <f t="shared" ref="A190:B192" si="21">A189</f>
+        <v>Facility throughput, capacity</v>
+      </c>
+      <c r="B190" t="str">
+        <f t="shared" si="21"/>
+        <v>Throughput (mass basis)</v>
+      </c>
+      <c r="C190" t="s">
+        <v>281</v>
+      </c>
+      <c r="D190" t="s">
+        <v>279</v>
+      </c>
+      <c r="F190">
+        <v>1.0160469999999999</v>
+      </c>
+    </row>
+    <row r="191" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A191" t="str">
+        <f t="shared" si="21"/>
+        <v>Facility throughput, capacity</v>
+      </c>
+      <c r="B191" t="str">
+        <f t="shared" si="21"/>
+        <v>Throughput (mass basis)</v>
+      </c>
+      <c r="C191" t="s">
+        <v>282</v>
+      </c>
+      <c r="D191" t="s">
+        <v>279</v>
+      </c>
+      <c r="F191">
+        <v>0.90718469999999996</v>
+      </c>
+    </row>
+    <row r="192" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A192" t="str">
+        <f t="shared" si="21"/>
+        <v>Facility throughput, capacity</v>
+      </c>
+      <c r="B192" t="str">
+        <f t="shared" si="21"/>
+        <v>Throughput (mass basis)</v>
+      </c>
+      <c r="C192" t="s">
+        <v>283</v>
+      </c>
+      <c r="D192" t="s">
+        <v>284</v>
+      </c>
+      <c r="F192">
+        <v>0.45359240000000001</v>
       </c>
     </row>
   </sheetData>

</xml_diff>